<commit_message>
Update ReleasePlan project folder
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
+++ b/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98D4764-1732-4802-8302-C8A0871F2B2E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE29F3E-5233-46E0-97AB-B5DE4E33BB99}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Abgeschlossen</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t xml:space="preserve">Powershellskript legt Musterordner mit Inhalten automatisch an </t>
+  </si>
+  <si>
+    <t>control.spInitialisiereDataFactory</t>
   </si>
 </sst>
 </file>
@@ -891,12 +894,12 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N323"/>
+  <dimension ref="A1:N324"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1178,7 @@
     <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
       <c r="D20" s="17" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
@@ -1187,7 +1190,7 @@
     <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C21" s="17"/>
       <c r="D21" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
@@ -1197,8 +1200,9 @@
       <c r="N21" s="33"/>
     </row>
     <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="17"/>
       <c r="D22" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
@@ -1208,7 +1212,9 @@
       <c r="N22" s="33"/>
     </row>
     <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
@@ -1217,72 +1223,70 @@
       <c r="N23" s="33"/>
     </row>
     <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="D24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="33"/>
+    </row>
+    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26">
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26">
         <v>43411</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="35"/>
-    </row>
-    <row r="25" spans="2:14" s="4" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="42"/>
-    </row>
-    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="35"/>
+    </row>
+    <row r="26" spans="2:14" s="4" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="38"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="42"/>
+    </row>
+    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <v>1</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I27" s="18">
         <v>0</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J27" s="18">
         <v>0</v>
       </c>
-      <c r="K26" s="18">
-        <f>I26/100*(100-J26)</f>
+      <c r="K27" s="18">
+        <f>I27/100*(100-J27)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="22" t="s">
+      <c r="L27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="36"/>
-    </row>
-    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="17" t="s">
+      <c r="M27" s="20"/>
+      <c r="N27" s="36"/>
+    </row>
+    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="33"/>
-    </row>
-    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -1292,7 +1296,9 @@
       <c r="N28" s="33"/>
     </row>
     <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="17"/>
+      <c r="C29" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -1300,7 +1306,8 @@
       <c r="M29" s="20"/>
       <c r="N29" s="33"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="17"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
@@ -1308,92 +1315,89 @@
       <c r="M30" s="20"/>
       <c r="N30" s="33"/>
     </row>
-    <row r="31" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="33"/>
+    </row>
+    <row r="32" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="34"/>
-    </row>
-    <row r="32" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="33"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="33"/>
+    </row>
+    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="35"/>
-    </row>
-    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="33"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="35"/>
     </row>
     <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="18">
-        <v>0</v>
-      </c>
-      <c r="J35" s="18">
-        <v>0</v>
-      </c>
-      <c r="K35" s="18">
-        <f>I35/100*(100-J35)</f>
-        <v>0</v>
-      </c>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
-      <c r="N35" s="36"/>
+      <c r="N35" s="33"/>
     </row>
     <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
+      <c r="B36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="18">
+        <v>0</v>
+      </c>
+      <c r="J36" s="18">
+        <v>0</v>
+      </c>
+      <c r="K36" s="18">
+        <f>I36/100*(100-J36)</f>
+        <v>0</v>
+      </c>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
       <c r="N36" s="36"/>
     </row>
     <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="C37" s="17" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1406,7 @@
       <c r="K37" s="18"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
-      <c r="N37" s="33"/>
+      <c r="N37" s="36"/>
     </row>
     <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C38" s="17" t="s">
@@ -1427,6 +1431,9 @@
       <c r="N39" s="33"/>
     </row>
     <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="18"/>
@@ -1435,18 +1442,16 @@
       <c r="N40" s="33"/>
     </row>
     <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="16"/>
-      <c r="C41" s="9"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20"/>
-      <c r="N41" s="36"/>
+      <c r="N41" s="33"/>
     </row>
     <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="15"/>
-      <c r="C42" s="17"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="9"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
@@ -1455,13 +1460,14 @@
       <c r="N42" s="36"/>
     </row>
     <row r="43" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="15"/>
       <c r="C43" s="17"/>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
       <c r="K43" s="18"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
-      <c r="N43" s="33"/>
+      <c r="N43" s="36"/>
     </row>
     <row r="44" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C44" s="17"/>
@@ -1490,7 +1496,7 @@
       <c r="M46" s="20"/>
       <c r="N46" s="33"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C47" s="17"/>
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
@@ -1499,71 +1505,69 @@
       <c r="M47" s="20"/>
       <c r="N47" s="33"/>
     </row>
-    <row r="48" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="29" t="s">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C48" s="17"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="33"/>
+    </row>
+    <row r="49" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="31"/>
-      <c r="N48" s="34"/>
-    </row>
-    <row r="49" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="33"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="34"/>
     </row>
     <row r="50" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="16" t="s">
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="33"/>
+    </row>
+    <row r="51" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I50" s="18">
+      <c r="I51" s="18">
         <v>5</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J51" s="18">
         <v>100</v>
       </c>
-      <c r="K50" s="18">
-        <f>I50/100*(100-J50)</f>
+      <c r="K51" s="18">
+        <f>I51/100*(100-J51)</f>
         <v>0</v>
       </c>
-      <c r="L50" s="20" t="s">
+      <c r="L51" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M50" s="20">
+      <c r="M51" s="20">
         <v>1</v>
       </c>
-      <c r="N50" s="36" t="s">
+      <c r="N51" s="36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="15"/>
-      <c r="C51" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="36"/>
-    </row>
     <row r="52" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="15"/>
       <c r="C52" s="17" t="s">
         <v>15</v>
       </c>
@@ -1572,7 +1576,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
-      <c r="N52" s="33"/>
+      <c r="N52" s="36"/>
     </row>
     <row r="53" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C53" s="17" t="s">
@@ -1597,6 +1601,9 @@
       <c r="N54" s="33"/>
     </row>
     <row r="55" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
@@ -1620,13 +1627,13 @@
       <c r="M57" s="20"/>
       <c r="N57" s="33"/>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-      <c r="N58" s="37"/>
+    <row r="58" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="33"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I59" s="19"/>
@@ -1634,6 +1641,7 @@
       <c r="K59" s="19"/>
       <c r="L59" s="21"/>
       <c r="M59" s="21"/>
+      <c r="N59" s="37"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I60" s="19"/>
@@ -2962,6 +2970,8 @@
       <c r="I249" s="19"/>
       <c r="J249" s="19"/>
       <c r="K249" s="19"/>
+      <c r="L249" s="21"/>
+      <c r="M249" s="21"/>
     </row>
     <row r="250" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I250" s="19"/>
@@ -3333,8 +3343,13 @@
       <c r="J323" s="19"/>
       <c r="K323" s="19"/>
     </row>
+    <row r="324" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I324" s="19"/>
+      <c r="J324" s="19"/>
+      <c r="K324" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M9:M10 M13:M23 M32:M1013 M29:M30">
+  <conditionalFormatting sqref="M9:M10 M13:M24 M33:M1014 M30:M31">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3342,7 +3357,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M31">
+  <conditionalFormatting sqref="M32">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3358,7 +3373,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26:M28">
+  <conditionalFormatting sqref="M27:M29">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3366,7 +3381,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:M25">
+  <conditionalFormatting sqref="M25:M26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update project folder, Failure report scripts
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
+++ b/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE29F3E-5233-46E0-97AB-B5DE4E33BB99}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13541108-7E7E-4FCF-A72A-6A60457B59E8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Abgeschlossen</t>
   </si>
@@ -156,6 +156,36 @@
   </si>
   <si>
     <t>control.spInitialisiereDataFactory</t>
+  </si>
+  <si>
+    <t>Release Projektordner 1.2</t>
+  </si>
+  <si>
+    <t>User Failure Report integrieren</t>
+  </si>
+  <si>
+    <t>Ordnerstruktur für User Failure Report generieren</t>
+  </si>
+  <si>
+    <t>..\08_Control\User Failure Report</t>
+  </si>
+  <si>
+    <t>..\08_Control\User Failure Report\Snippets</t>
+  </si>
+  <si>
+    <t>Basis SQL-Skripte um Prozedur control.spCustomFailureReport zu generieren</t>
+  </si>
+  <si>
+    <t>01_Header.sql</t>
+  </si>
+  <si>
+    <t>02_Footer.sql</t>
+  </si>
+  <si>
+    <t>001_Sample UserFailureReport Snippet.sql</t>
+  </si>
+  <si>
+    <t>Powershell-Skript zur Generierung Prozedur ontrol.spCustomFailureReport</t>
   </si>
 </sst>
 </file>
@@ -310,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -422,11 +452,62 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -894,12 +975,12 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N324"/>
+  <dimension ref="A1:N336"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1388,7 @@
       <c r="N29" s="33"/>
     </row>
     <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="17"/>
+      <c r="C30" s="17"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
@@ -1315,57 +1396,74 @@
       <c r="M30" s="20"/>
       <c r="N30" s="33"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="33"/>
-    </row>
-    <row r="32" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="34"/>
-    </row>
-    <row r="33" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="20"/>
+    <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26">
+        <v>43412</v>
+      </c>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="35"/>
+    </row>
+    <row r="32" spans="2:14" s="4" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="38"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="42"/>
+    </row>
+    <row r="33" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="16">
+        <v>1</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="18">
+        <v>0</v>
+      </c>
+      <c r="J33" s="18">
+        <v>0</v>
+      </c>
+      <c r="K33" s="18">
+        <f>I33/100*(100-J33)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="M33" s="20"/>
-      <c r="N33" s="33"/>
-    </row>
-    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="35"/>
-    </row>
-    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="N33" s="36"/>
+    </row>
+    <row r="34" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="15"/>
+      <c r="C34" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="33"/>
+    </row>
+    <row r="35" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
@@ -1373,44 +1471,31 @@
       <c r="M35" s="20"/>
       <c r="N35" s="33"/>
     </row>
-    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="18">
-        <v>0</v>
-      </c>
-      <c r="J36" s="18">
-        <v>0</v>
-      </c>
-      <c r="K36" s="18">
-        <f>I36/100*(100-J36)</f>
-        <v>0</v>
-      </c>
+    <row r="36" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
-      <c r="N36" s="36"/>
-    </row>
-    <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="N36" s="33"/>
+    </row>
+    <row r="37" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="17" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
-      <c r="N37" s="36"/>
-    </row>
-    <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="17" t="s">
-        <v>12</v>
+      <c r="N37" s="33"/>
+    </row>
+    <row r="38" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="49" t="s">
+        <v>45</v>
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
@@ -1419,9 +1504,9 @@
       <c r="M38" s="20"/>
       <c r="N38" s="33"/>
     </row>
-    <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="17" t="s">
-        <v>12</v>
+    <row r="39" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="49" t="s">
+        <v>46</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
@@ -1430,9 +1515,9 @@
       <c r="M39" s="20"/>
       <c r="N39" s="33"/>
     </row>
-    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="17" t="s">
-        <v>12</v>
+    <row r="40" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="49" t="s">
+        <v>47</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
@@ -1441,7 +1526,10 @@
       <c r="M40" s="20"/>
       <c r="N40" s="33"/>
     </row>
-    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
@@ -1449,37 +1537,41 @@
       <c r="M41" s="20"/>
       <c r="N41" s="33"/>
     </row>
-    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="16"/>
-      <c r="C42" s="9"/>
+    <row r="42" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="17"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
-      <c r="N42" s="36"/>
-    </row>
-    <row r="43" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="15"/>
-      <c r="C43" s="17"/>
+      <c r="N42" s="33"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
       <c r="K43" s="18"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
-      <c r="N43" s="36"/>
-    </row>
-    <row r="44" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="17"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="33"/>
+      <c r="N43" s="33"/>
+    </row>
+    <row r="44" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="34"/>
     </row>
     <row r="45" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="17"/>
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
       <c r="K45" s="18"/>
@@ -1488,16 +1580,23 @@
       <c r="N45" s="33"/>
     </row>
     <row r="46" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="17"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="33"/>
+      <c r="B46" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="35"/>
     </row>
     <row r="47" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="17"/>
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
@@ -1505,33 +1604,45 @@
       <c r="M47" s="20"/>
       <c r="N47" s="33"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C48" s="17"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
+    <row r="48" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="18">
+        <v>0</v>
+      </c>
+      <c r="J48" s="18">
+        <v>0</v>
+      </c>
+      <c r="K48" s="18">
+        <f>I48/100*(100-J48)</f>
+        <v>0</v>
+      </c>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
-      <c r="N48" s="33"/>
-    </row>
-    <row r="49" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="31"/>
-      <c r="N49" s="34"/>
+      <c r="N48" s="36"/>
+    </row>
+    <row r="49" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="36"/>
     </row>
     <row r="50" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
@@ -1540,48 +1651,28 @@
       <c r="N50" s="33"/>
     </row>
     <row r="51" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="18">
-        <v>5</v>
-      </c>
-      <c r="J51" s="18">
-        <v>100</v>
-      </c>
-      <c r="K51" s="18">
-        <f>I51/100*(100-J51)</f>
-        <v>0</v>
-      </c>
-      <c r="L51" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M51" s="20">
-        <v>1</v>
-      </c>
-      <c r="N51" s="36" t="s">
-        <v>5</v>
-      </c>
+      <c r="C51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="33"/>
     </row>
     <row r="52" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
       <c r="C52" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
-      <c r="N52" s="36"/>
+      <c r="N52" s="33"/>
     </row>
     <row r="53" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="17" t="s">
-        <v>15</v>
-      </c>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
@@ -1590,28 +1681,27 @@
       <c r="N53" s="33"/>
     </row>
     <row r="54" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="17" t="s">
-        <v>15</v>
-      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="9"/>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
-      <c r="N54" s="33"/>
+      <c r="N54" s="36"/>
     </row>
     <row r="55" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="17" t="s">
-        <v>15</v>
-      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="17"/>
       <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
-      <c r="N55" s="33"/>
+      <c r="N55" s="36"/>
     </row>
     <row r="56" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="17"/>
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
@@ -1620,6 +1710,7 @@
       <c r="N56" s="33"/>
     </row>
     <row r="57" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="17"/>
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
@@ -1628,6 +1719,7 @@
       <c r="N57" s="33"/>
     </row>
     <row r="58" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="17"/>
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
@@ -1635,155 +1727,210 @@
       <c r="M58" s="20"/>
       <c r="N58" s="33"/>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="21"/>
-      <c r="M59" s="21"/>
-      <c r="N59" s="37"/>
+    <row r="59" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="17"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="33"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I62" s="19"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="21"/>
-    </row>
-    <row r="65" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
-    </row>
-    <row r="66" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
-    </row>
-    <row r="67" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="21"/>
-      <c r="M67" s="21"/>
-    </row>
-    <row r="68" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="19"/>
-      <c r="L68" s="21"/>
-      <c r="M68" s="21"/>
-    </row>
-    <row r="69" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
-      <c r="K69" s="19"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="21"/>
-    </row>
-    <row r="70" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
-      <c r="K70" s="19"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="21"/>
-    </row>
-    <row r="71" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="C60" s="17"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="33"/>
+    </row>
+    <row r="61" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
+      <c r="L61" s="31"/>
+      <c r="M61" s="31"/>
+      <c r="N61" s="34"/>
+    </row>
+    <row r="62" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="33"/>
+    </row>
+    <row r="63" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="18">
+        <v>5</v>
+      </c>
+      <c r="J63" s="18">
+        <v>100</v>
+      </c>
+      <c r="K63" s="18">
+        <f>I63/100*(100-J63)</f>
+        <v>0</v>
+      </c>
+      <c r="L63" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M63" s="20">
+        <v>1</v>
+      </c>
+      <c r="N63" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="15"/>
+      <c r="C64" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="36"/>
+    </row>
+    <row r="65" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="33"/>
+    </row>
+    <row r="66" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="33"/>
+    </row>
+    <row r="67" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="20"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="33"/>
+    </row>
+    <row r="68" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="33"/>
+    </row>
+    <row r="69" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="20"/>
+      <c r="N69" s="33"/>
+    </row>
+    <row r="70" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="33"/>
+    </row>
+    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I71" s="19"/>
       <c r="J71" s="19"/>
       <c r="K71" s="19"/>
       <c r="L71" s="21"/>
       <c r="M71" s="21"/>
-    </row>
-    <row r="72" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="37"/>
+    </row>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I72" s="19"/>
       <c r="J72" s="19"/>
       <c r="K72" s="19"/>
       <c r="L72" s="21"/>
       <c r="M72" s="21"/>
     </row>
-    <row r="73" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I73" s="19"/>
       <c r="J73" s="19"/>
       <c r="K73" s="19"/>
       <c r="L73" s="21"/>
       <c r="M73" s="21"/>
     </row>
-    <row r="74" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I74" s="19"/>
       <c r="J74" s="19"/>
       <c r="K74" s="19"/>
       <c r="L74" s="21"/>
       <c r="M74" s="21"/>
     </row>
-    <row r="75" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I75" s="19"/>
       <c r="J75" s="19"/>
       <c r="K75" s="19"/>
       <c r="L75" s="21"/>
       <c r="M75" s="21"/>
     </row>
-    <row r="76" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
       <c r="K76" s="19"/>
       <c r="L76" s="21"/>
       <c r="M76" s="21"/>
     </row>
-    <row r="77" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I77" s="19"/>
       <c r="J77" s="19"/>
       <c r="K77" s="19"/>
       <c r="L77" s="21"/>
       <c r="M77" s="21"/>
     </row>
-    <row r="78" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
       <c r="K78" s="19"/>
       <c r="L78" s="21"/>
       <c r="M78" s="21"/>
     </row>
-    <row r="79" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I79" s="19"/>
       <c r="J79" s="19"/>
       <c r="K79" s="19"/>
       <c r="L79" s="21"/>
       <c r="M79" s="21"/>
     </row>
-    <row r="80" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
       <c r="K80" s="19"/>
@@ -2977,113 +3124,137 @@
       <c r="I250" s="19"/>
       <c r="J250" s="19"/>
       <c r="K250" s="19"/>
+      <c r="L250" s="21"/>
+      <c r="M250" s="21"/>
     </row>
     <row r="251" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I251" s="19"/>
       <c r="J251" s="19"/>
       <c r="K251" s="19"/>
+      <c r="L251" s="21"/>
+      <c r="M251" s="21"/>
     </row>
     <row r="252" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I252" s="19"/>
       <c r="J252" s="19"/>
       <c r="K252" s="19"/>
+      <c r="L252" s="21"/>
+      <c r="M252" s="21"/>
     </row>
     <row r="253" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I253" s="19"/>
       <c r="J253" s="19"/>
       <c r="K253" s="19"/>
+      <c r="L253" s="21"/>
+      <c r="M253" s="21"/>
     </row>
     <row r="254" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I254" s="19"/>
       <c r="J254" s="19"/>
       <c r="K254" s="19"/>
+      <c r="L254" s="21"/>
+      <c r="M254" s="21"/>
     </row>
     <row r="255" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I255" s="19"/>
       <c r="J255" s="19"/>
       <c r="K255" s="19"/>
+      <c r="L255" s="21"/>
+      <c r="M255" s="21"/>
     </row>
     <row r="256" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I256" s="19"/>
       <c r="J256" s="19"/>
       <c r="K256" s="19"/>
-    </row>
-    <row r="257" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L256" s="21"/>
+      <c r="M256" s="21"/>
+    </row>
+    <row r="257" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I257" s="19"/>
       <c r="J257" s="19"/>
       <c r="K257" s="19"/>
-    </row>
-    <row r="258" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L257" s="21"/>
+      <c r="M257" s="21"/>
+    </row>
+    <row r="258" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I258" s="19"/>
       <c r="J258" s="19"/>
       <c r="K258" s="19"/>
-    </row>
-    <row r="259" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L258" s="21"/>
+      <c r="M258" s="21"/>
+    </row>
+    <row r="259" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I259" s="19"/>
       <c r="J259" s="19"/>
       <c r="K259" s="19"/>
-    </row>
-    <row r="260" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L259" s="21"/>
+      <c r="M259" s="21"/>
+    </row>
+    <row r="260" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I260" s="19"/>
       <c r="J260" s="19"/>
       <c r="K260" s="19"/>
-    </row>
-    <row r="261" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L260" s="21"/>
+      <c r="M260" s="21"/>
+    </row>
+    <row r="261" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I261" s="19"/>
       <c r="J261" s="19"/>
       <c r="K261" s="19"/>
-    </row>
-    <row r="262" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L261" s="21"/>
+      <c r="M261" s="21"/>
+    </row>
+    <row r="262" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I262" s="19"/>
       <c r="J262" s="19"/>
       <c r="K262" s="19"/>
     </row>
-    <row r="263" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I263" s="19"/>
       <c r="J263" s="19"/>
       <c r="K263" s="19"/>
     </row>
-    <row r="264" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I264" s="19"/>
       <c r="J264" s="19"/>
       <c r="K264" s="19"/>
     </row>
-    <row r="265" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I265" s="19"/>
       <c r="J265" s="19"/>
       <c r="K265" s="19"/>
     </row>
-    <row r="266" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I266" s="19"/>
       <c r="J266" s="19"/>
       <c r="K266" s="19"/>
     </row>
-    <row r="267" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I267" s="19"/>
       <c r="J267" s="19"/>
       <c r="K267" s="19"/>
     </row>
-    <row r="268" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I268" s="19"/>
       <c r="J268" s="19"/>
       <c r="K268" s="19"/>
     </row>
-    <row r="269" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I269" s="19"/>
       <c r="J269" s="19"/>
       <c r="K269" s="19"/>
     </row>
-    <row r="270" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I270" s="19"/>
       <c r="J270" s="19"/>
       <c r="K270" s="19"/>
     </row>
-    <row r="271" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I271" s="19"/>
       <c r="J271" s="19"/>
       <c r="K271" s="19"/>
     </row>
-    <row r="272" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I272" s="19"/>
       <c r="J272" s="19"/>
       <c r="K272" s="19"/>
@@ -3348,8 +3519,84 @@
       <c r="J324" s="19"/>
       <c r="K324" s="19"/>
     </row>
+    <row r="325" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I325" s="19"/>
+      <c r="J325" s="19"/>
+      <c r="K325" s="19"/>
+    </row>
+    <row r="326" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I326" s="19"/>
+      <c r="J326" s="19"/>
+      <c r="K326" s="19"/>
+    </row>
+    <row r="327" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I327" s="19"/>
+      <c r="J327" s="19"/>
+      <c r="K327" s="19"/>
+    </row>
+    <row r="328" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I328" s="19"/>
+      <c r="J328" s="19"/>
+      <c r="K328" s="19"/>
+    </row>
+    <row r="329" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I329" s="19"/>
+      <c r="J329" s="19"/>
+      <c r="K329" s="19"/>
+    </row>
+    <row r="330" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I330" s="19"/>
+      <c r="J330" s="19"/>
+      <c r="K330" s="19"/>
+    </row>
+    <row r="331" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I331" s="19"/>
+      <c r="J331" s="19"/>
+      <c r="K331" s="19"/>
+    </row>
+    <row r="332" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I332" s="19"/>
+      <c r="J332" s="19"/>
+      <c r="K332" s="19"/>
+    </row>
+    <row r="333" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I333" s="19"/>
+      <c r="J333" s="19"/>
+      <c r="K333" s="19"/>
+    </row>
+    <row r="334" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I334" s="19"/>
+      <c r="J334" s="19"/>
+      <c r="K334" s="19"/>
+    </row>
+    <row r="335" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I335" s="19"/>
+      <c r="J335" s="19"/>
+      <c r="K335" s="19"/>
+    </row>
+    <row r="336" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I336" s="19"/>
+      <c r="J336" s="19"/>
+      <c r="K336" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M9:M10 M13:M24 M33:M1014 M30:M31">
+  <conditionalFormatting sqref="M9:M10 M13:M24 M45:M1026 M42:M43">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M44">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M12">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3357,7 +3604,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M32">
+  <conditionalFormatting sqref="M27:M30 M36:M41">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3365,7 +3612,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M12">
+  <conditionalFormatting sqref="M25:M26">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3373,7 +3620,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27:M29">
+  <conditionalFormatting sqref="M33:M35">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3381,7 +3628,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:M26">
+  <conditionalFormatting sqref="M31:M32">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
separate Dateien für API und Tabellen, Header vor Tabellen
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
+++ b/8. Harmonising standards/01_Project organisation/02_Project Folder/ReleasePlan_ProjectFolder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465BC7A1-312E-4BCC-B0FF-3A5A5083A3DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A78ABD1-007D-4BF9-8A69-DAC4E8BC4BD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Abgeschlossen</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Powershell für Konkatenierung getrennt für API und Tabellen</t>
+  </si>
+  <si>
+    <t>Release Projektordner 1.3</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,55 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -978,12 +1029,12 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N336"/>
+  <dimension ref="A1:N339"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1541,7 +1592,7 @@
       <c r="N41" s="33"/>
     </row>
     <row r="42" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="17"/>
+      <c r="C42" s="17"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
@@ -1549,103 +1600,108 @@
       <c r="M42" s="20"/>
       <c r="N42" s="33"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="33"/>
-    </row>
-    <row r="44" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+    <row r="43" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="26">
+        <v>43448</v>
+      </c>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="35"/>
+    </row>
+    <row r="44" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="17"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="33"/>
+    </row>
+    <row r="45" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="16">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="18">
+        <v>0</v>
+      </c>
+      <c r="J45" s="18">
+        <v>0</v>
+      </c>
+      <c r="K45" s="18">
+        <f>I45/100*(100-J45)</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="20"/>
+      <c r="N45" s="36"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="33"/>
+    </row>
+    <row r="47" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="34"/>
-    </row>
-    <row r="45" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="33"/>
-    </row>
-    <row r="46" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="35"/>
-    </row>
-    <row r="47" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="33"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="34"/>
     </row>
     <row r="48" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48" s="18">
-        <v>0</v>
-      </c>
-      <c r="J48" s="18">
-        <v>0</v>
-      </c>
-      <c r="K48" s="18">
-        <f>I48/100*(100-J48)</f>
-        <v>0</v>
-      </c>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
-      <c r="N48" s="36"/>
+      <c r="N48" s="33"/>
     </row>
     <row r="49" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="36"/>
+      <c r="B49" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="35"/>
     </row>
     <row r="50" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="17" t="s">
-        <v>12</v>
-      </c>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
@@ -1654,17 +1710,30 @@
       <c r="N50" s="33"/>
     </row>
     <row r="51" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
+      <c r="B51" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="18">
+        <v>0</v>
+      </c>
+      <c r="J51" s="18">
+        <v>0</v>
+      </c>
+      <c r="K51" s="18">
+        <f>I51/100*(100-J51)</f>
+        <v>0</v>
+      </c>
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
-      <c r="N51" s="33"/>
+      <c r="N51" s="36"/>
     </row>
     <row r="52" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="C52" s="17" t="s">
         <v>12</v>
       </c>
@@ -1673,9 +1742,12 @@
       <c r="K52" s="18"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
-      <c r="N52" s="33"/>
+      <c r="N52" s="36"/>
     </row>
     <row r="53" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
@@ -1684,27 +1756,28 @@
       <c r="N53" s="33"/>
     </row>
     <row r="54" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="16"/>
-      <c r="C54" s="9"/>
+      <c r="C54" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
-      <c r="N54" s="36"/>
+      <c r="N54" s="33"/>
     </row>
     <row r="55" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="15"/>
-      <c r="C55" s="17"/>
+      <c r="C55" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
-      <c r="N55" s="36"/>
+      <c r="N55" s="33"/>
     </row>
     <row r="56" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="17"/>
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
@@ -1713,22 +1786,24 @@
       <c r="N56" s="33"/>
     </row>
     <row r="57" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="17"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="9"/>
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
       <c r="L57" s="20"/>
       <c r="M57" s="20"/>
-      <c r="N57" s="33"/>
+      <c r="N57" s="36"/>
     </row>
     <row r="58" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="15"/>
       <c r="C58" s="17"/>
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20"/>
-      <c r="N58" s="33"/>
+      <c r="N58" s="36"/>
     </row>
     <row r="59" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C59" s="17"/>
@@ -1739,7 +1814,7 @@
       <c r="M59" s="20"/>
       <c r="N59" s="33"/>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C60" s="17"/>
       <c r="I60" s="18"/>
       <c r="J60" s="18"/>
@@ -1748,24 +1823,17 @@
       <c r="M60" s="20"/>
       <c r="N60" s="33"/>
     </row>
-    <row r="61" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-      <c r="L61" s="31"/>
-      <c r="M61" s="31"/>
-      <c r="N61" s="34"/>
+    <row r="61" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="17"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="33"/>
     </row>
     <row r="62" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="17"/>
       <c r="I62" s="18"/>
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
@@ -1773,49 +1841,33 @@
       <c r="M62" s="20"/>
       <c r="N62" s="33"/>
     </row>
-    <row r="63" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I63" s="18">
-        <v>5</v>
-      </c>
-      <c r="J63" s="18">
-        <v>100</v>
-      </c>
-      <c r="K63" s="18">
-        <f>I63/100*(100-J63)</f>
-        <v>0</v>
-      </c>
-      <c r="L63" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M63" s="20">
-        <v>1</v>
-      </c>
-      <c r="N63" s="36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-      <c r="C64" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="20"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="36"/>
-    </row>
-    <row r="65" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C63" s="17"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="33"/>
+    </row>
+    <row r="64" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="30"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="31"/>
+      <c r="M64" s="31"/>
+      <c r="N64" s="34"/>
+    </row>
+    <row r="65" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I65" s="18"/>
       <c r="J65" s="18"/>
       <c r="K65" s="18"/>
@@ -1823,18 +1875,35 @@
       <c r="M65" s="20"/>
       <c r="N65" s="33"/>
     </row>
-    <row r="66" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18"/>
-      <c r="L66" s="20"/>
-      <c r="M66" s="20"/>
-      <c r="N66" s="33"/>
-    </row>
-    <row r="67" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="18">
+        <v>5</v>
+      </c>
+      <c r="J66" s="18">
+        <v>100</v>
+      </c>
+      <c r="K66" s="18">
+        <f>I66/100*(100-J66)</f>
+        <v>0</v>
+      </c>
+      <c r="L66" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M66" s="20">
+        <v>1</v>
+      </c>
+      <c r="N66" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="15"/>
       <c r="C67" s="17" t="s">
         <v>15</v>
       </c>
@@ -1843,9 +1912,12 @@
       <c r="K67" s="18"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
-      <c r="N67" s="33"/>
-    </row>
-    <row r="68" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="N67" s="36"/>
+    </row>
+    <row r="68" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="I68" s="18"/>
       <c r="J68" s="18"/>
       <c r="K68" s="18"/>
@@ -1853,7 +1925,10 @@
       <c r="M68" s="20"/>
       <c r="N68" s="33"/>
     </row>
-    <row r="69" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="I69" s="18"/>
       <c r="J69" s="18"/>
       <c r="K69" s="18"/>
@@ -1861,7 +1936,10 @@
       <c r="M69" s="20"/>
       <c r="N69" s="33"/>
     </row>
-    <row r="70" spans="3:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="I70" s="18"/>
       <c r="J70" s="18"/>
       <c r="K70" s="18"/>
@@ -1869,74 +1947,75 @@
       <c r="M70" s="20"/>
       <c r="N70" s="33"/>
     </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="I71" s="19"/>
-      <c r="J71" s="19"/>
-      <c r="K71" s="19"/>
-      <c r="L71" s="21"/>
-      <c r="M71" s="21"/>
-      <c r="N71" s="37"/>
-    </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C72" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
-      <c r="K72" s="19"/>
-      <c r="L72" s="21"/>
-      <c r="M72" s="21"/>
-    </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="I73" s="19"/>
-      <c r="J73" s="19"/>
-      <c r="K73" s="19"/>
-      <c r="L73" s="21"/>
-      <c r="M73" s="21"/>
-    </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="20"/>
+      <c r="M71" s="20"/>
+      <c r="N71" s="33"/>
+    </row>
+    <row r="72" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="20"/>
+      <c r="N72" s="33"/>
+    </row>
+    <row r="73" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="20"/>
+      <c r="N73" s="33"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I74" s="19"/>
       <c r="J74" s="19"/>
       <c r="K74" s="19"/>
       <c r="L74" s="21"/>
       <c r="M74" s="21"/>
-    </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N74" s="37"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C75" s="9"/>
       <c r="I75" s="19"/>
       <c r="J75" s="19"/>
       <c r="K75" s="19"/>
       <c r="L75" s="21"/>
       <c r="M75" s="21"/>
     </row>
-    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
       <c r="K76" s="19"/>
       <c r="L76" s="21"/>
       <c r="M76" s="21"/>
     </row>
-    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I77" s="19"/>
       <c r="J77" s="19"/>
       <c r="K77" s="19"/>
       <c r="L77" s="21"/>
       <c r="M77" s="21"/>
     </row>
-    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
       <c r="K78" s="19"/>
       <c r="L78" s="21"/>
       <c r="M78" s="21"/>
     </row>
-    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I79" s="19"/>
       <c r="J79" s="19"/>
       <c r="K79" s="19"/>
       <c r="L79" s="21"/>
       <c r="M79" s="21"/>
     </row>
-    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
       <c r="K80" s="19"/>
@@ -3214,16 +3293,22 @@
       <c r="I262" s="19"/>
       <c r="J262" s="19"/>
       <c r="K262" s="19"/>
+      <c r="L262" s="21"/>
+      <c r="M262" s="21"/>
     </row>
     <row r="263" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I263" s="19"/>
       <c r="J263" s="19"/>
       <c r="K263" s="19"/>
+      <c r="L263" s="21"/>
+      <c r="M263" s="21"/>
     </row>
     <row r="264" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I264" s="19"/>
       <c r="J264" s="19"/>
       <c r="K264" s="19"/>
+      <c r="L264" s="21"/>
+      <c r="M264" s="21"/>
     </row>
     <row r="265" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I265" s="19"/>
@@ -3585,8 +3670,39 @@
       <c r="J336" s="19"/>
       <c r="K336" s="19"/>
     </row>
+    <row r="337" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I337" s="19"/>
+      <c r="J337" s="19"/>
+      <c r="K337" s="19"/>
+    </row>
+    <row r="338" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I338" s="19"/>
+      <c r="J338" s="19"/>
+      <c r="K338" s="19"/>
+    </row>
+    <row r="339" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I339" s="19"/>
+      <c r="J339" s="19"/>
+      <c r="K339" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M9:M10 M13:M24 M45:M1026 M42:M43">
+  <conditionalFormatting sqref="M9:M10 M13:M24 M48:M1029 M46">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M47">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M12">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3594,7 +3710,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M44">
+  <conditionalFormatting sqref="M27:M30 M36:M42 M44">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3602,7 +3718,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M12">
+  <conditionalFormatting sqref="M25:M26">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3610,7 +3726,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27:M30 M36:M41">
+  <conditionalFormatting sqref="M33:M35">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3618,7 +3734,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:M26">
+  <conditionalFormatting sqref="M31:M32">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3626,7 +3742,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33:M35">
+  <conditionalFormatting sqref="M43">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3634,7 +3750,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M31:M32">
+  <conditionalFormatting sqref="M45">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>